<commit_message>
Updating missing files, and updated configs for the UC2 configurator
</commit_message>
<xml_diff>
--- a/DOCUMENTS/UC2-Configurator/UC2_ReadyToUse_Boxes_Modules_Parts.xlsx
+++ b/DOCUMENTS/UC2-Configurator/UC2_ReadyToUse_Boxes_Modules_Parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bene/Dropbox/Dokumente/Promotion/PROJECTS/UC2-GIT/DOCUMENTS/UC2-Configurator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F465551-CFF3-F84B-9BA2-C39E3E5A2CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A0E37A-A4BA-C14B-A073-C6ADC5A6A60E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="27880" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete overview" sheetId="1" r:id="rId1"/>
@@ -731,19 +731,10 @@
     <t>30_Z_Stage_Adapterplate</t>
   </si>
   <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_v2/STL/30_Z_Stage_Adapterplate_11.stl</t>
-  </si>
-  <si>
     <t>30_Z_Stage_Fluomodule</t>
   </si>
   <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_v2/STL/30_Z_Stage_Fluomodule_12.stl</t>
-  </si>
-  <si>
     <t>40_XY_Stage_Clamp_Slide</t>
-  </si>
-  <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_v2/STL/40_XY_Stage_Clamp_Slide_9.stl</t>
   </si>
   <si>
     <t>ASSEMBLY_CUBE_Z-stage_mechanical</t>
@@ -752,43 +743,19 @@
     <t>https://github.com/bionanoimaging/UC2-GIT/tree/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2</t>
   </si>
   <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_10_Cube_2x1_v2_5.stl</t>
-  </si>
-  <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_10_Lid_el_2x1_v2_6.stl</t>
-  </si>
-  <si>
     <t xml:space="preserve">The linearflexure mechanism of the Z-stage is used for precise focussing of the microscope objective. Mechanical only. </t>
-  </si>
-  <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_20_focus_inlet_linearflexure_v0_1.stl</t>
-  </si>
-  <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_30_focus_inlet_objective_mount_v7_7.stl</t>
   </si>
   <si>
     <t>20_focus_inlet_plate_bottom</t>
   </si>
   <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_20_focus_inlet_plate_bottom_2.stl</t>
-  </si>
-  <si>
     <t>20_focus_inlet_plate_top</t>
-  </si>
-  <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_20_focus_inlet_plate_top_3.stl</t>
   </si>
   <si>
     <t>00_large_gear</t>
   </si>
   <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_00_large_gear_4.stl</t>
-  </si>
-  <si>
     <t>30_Z_Stage_Sampleplate</t>
-  </si>
-  <si>
-    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_30_Z_Stage_Sampleplate_8.stl</t>
   </si>
   <si>
     <t>ASSEMBLY_CUBE_Circular_Aperture</t>
@@ -1963,6 +1930,39 @@
   <si>
     <t>ASSEMBLY_Baseplate 4x11</t>
   </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_v2/STL/30_Z_Stage_Adapterplate.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_v2/STL/30_Z_Stage_Fluomodule.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_v2/STL/40_XY_Stage_Clamp_Slide.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_10_Cube_2x1_v2.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_10_Lid_el_2x1_v2.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_20_focus_inlet_linearflexure_v0.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_30_focus_inlet_objective_mount_v7.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_20_focus_inlet_plate_bottom.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_20_focus_inlet_plate_top.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_00_large_gear.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/bionanoimaging/UC2-GIT/blob/master/CAD/ASSEMBLY_CUBE_Z-STAGE_mechanical_v2/STL/Assembly_Z-Focus_Linearbearing_mechanical_v0_30_Z_Stage_Sampleplate.stl</t>
+  </si>
 </sst>
 </file>
 
@@ -2701,7 +2701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3017,6 +3017,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -3342,7 +3343,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -3408,40 +3409,40 @@
         <v>5</v>
       </c>
       <c r="K2" s="191" t="s">
+        <v>590</v>
+      </c>
+      <c r="L2" s="191" t="s">
+        <v>591</v>
+      </c>
+      <c r="M2" s="192" t="s">
+        <v>592</v>
+      </c>
+      <c r="N2" s="192" t="s">
+        <v>593</v>
+      </c>
+      <c r="O2" s="191" t="s">
+        <v>594</v>
+      </c>
+      <c r="P2" s="191" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q2" s="191" t="s">
+        <v>596</v>
+      </c>
+      <c r="R2" s="191" t="s">
+        <v>597</v>
+      </c>
+      <c r="S2" s="191" t="s">
+        <v>598</v>
+      </c>
+      <c r="T2" s="191" t="s">
+        <v>599</v>
+      </c>
+      <c r="U2" s="191" t="s">
+        <v>600</v>
+      </c>
+      <c r="V2" s="191" t="s">
         <v>601</v>
-      </c>
-      <c r="L2" s="191" t="s">
-        <v>602</v>
-      </c>
-      <c r="M2" s="192" t="s">
-        <v>603</v>
-      </c>
-      <c r="N2" s="192" t="s">
-        <v>604</v>
-      </c>
-      <c r="O2" s="191" t="s">
-        <v>605</v>
-      </c>
-      <c r="P2" s="191" t="s">
-        <v>606</v>
-      </c>
-      <c r="Q2" s="191" t="s">
-        <v>607</v>
-      </c>
-      <c r="R2" s="191" t="s">
-        <v>608</v>
-      </c>
-      <c r="S2" s="191" t="s">
-        <v>609</v>
-      </c>
-      <c r="T2" s="191" t="s">
-        <v>610</v>
-      </c>
-      <c r="U2" s="191" t="s">
-        <v>611</v>
-      </c>
-      <c r="V2" s="191" t="s">
-        <v>612</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
@@ -3725,7 +3726,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>633</v>
+        <v>622</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -3792,7 +3793,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
       <c r="D8" s="26">
         <v>1</v>
@@ -3874,7 +3875,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>614</v>
+        <v>603</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -3941,7 +3942,7 @@
         <v>62</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="D11" s="26">
         <v>1</v>
@@ -4023,7 +4024,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -4090,7 +4091,7 @@
         <v>62</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="D14" s="26">
         <v>1</v>
@@ -4172,7 +4173,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -4320,7 +4321,7 @@
       <c r="A19" s="54"/>
       <c r="B19" s="55"/>
       <c r="C19" s="25" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="D19" s="50">
         <v>0</v>
@@ -4359,7 +4360,7 @@
       <c r="A20" s="54"/>
       <c r="B20" s="57"/>
       <c r="C20" s="58" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="D20" s="59">
         <v>0</v>
@@ -4466,7 +4467,7 @@
         <v>76</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D22" s="50"/>
       <c r="E22" s="50">
@@ -4733,7 +4734,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D28" s="50"/>
       <c r="E28" s="50">
@@ -4922,7 +4923,7 @@
         <v>95</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D32" s="50"/>
       <c r="E32" s="50">
@@ -5043,7 +5044,7 @@
       <c r="A35" s="54"/>
       <c r="B35" s="57"/>
       <c r="C35" s="64" t="s">
-        <v>621</v>
+        <v>610</v>
       </c>
       <c r="D35" s="65">
         <v>0</v>
@@ -5228,10 +5229,10 @@
     <row r="39" spans="1:27" ht="16">
       <c r="A39" s="5"/>
       <c r="B39" s="63" t="s">
-        <v>622</v>
+        <v>611</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="D39" s="50">
         <v>0</v>
@@ -5309,7 +5310,7 @@
       <c r="A41" s="54"/>
       <c r="B41" s="55"/>
       <c r="C41" s="25" t="s">
-        <v>623</v>
+        <v>612</v>
       </c>
       <c r="D41" s="50">
         <v>0</v>
@@ -5533,7 +5534,7 @@
         <v>117</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D46" s="50"/>
       <c r="E46" s="50">
@@ -5954,7 +5955,7 @@
         <v>133</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D56" s="50"/>
       <c r="E56" s="50">
@@ -6114,7 +6115,7 @@
       <c r="A60" s="54"/>
       <c r="B60" s="57"/>
       <c r="C60" s="64" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
       <c r="D60" s="65">
         <v>0</v>
@@ -6221,7 +6222,7 @@
         <v>143</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D62" s="50"/>
       <c r="E62" s="50">
@@ -6410,7 +6411,7 @@
         <v>150</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D66" s="50"/>
       <c r="E66" s="50">
@@ -6638,7 +6639,7 @@
         <v>150</v>
       </c>
       <c r="C71" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D71" s="50"/>
       <c r="E71" s="50">
@@ -6866,7 +6867,7 @@
         <v>150</v>
       </c>
       <c r="C76" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D76" s="50"/>
       <c r="E76" s="50">
@@ -7027,7 +7028,7 @@
         <v>15</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
@@ -7094,7 +7095,7 @@
         <v>150</v>
       </c>
       <c r="C81" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D81" s="50"/>
       <c r="E81" s="50">
@@ -7174,7 +7175,7 @@
       <c r="A83" s="54"/>
       <c r="B83" s="57"/>
       <c r="C83" s="64" t="s">
-        <v>626</v>
+        <v>615</v>
       </c>
       <c r="D83" s="65">
         <v>0</v>
@@ -7281,7 +7282,7 @@
         <v>150</v>
       </c>
       <c r="C85" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D85" s="50"/>
       <c r="E85" s="50">
@@ -7509,7 +7510,7 @@
         <v>170</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D90" s="50"/>
       <c r="E90" s="50">
@@ -7591,7 +7592,7 @@
         <v>173</v>
       </c>
       <c r="C92" s="64" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
       <c r="D92" s="65">
         <v>0</v>
@@ -7698,7 +7699,7 @@
         <v>176</v>
       </c>
       <c r="C94" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D94" s="50"/>
       <c r="E94" s="50">
@@ -7780,7 +7781,7 @@
         <v>179</v>
       </c>
       <c r="C96" s="25" t="s">
-        <v>628</v>
+        <v>617</v>
       </c>
       <c r="D96" s="50">
         <v>0</v>
@@ -7817,7 +7818,7 @@
       <c r="A97" s="54"/>
       <c r="B97" s="55"/>
       <c r="C97" s="25" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
       <c r="D97" s="50">
         <v>0</v>
@@ -7856,7 +7857,7 @@
       <c r="A98" s="54"/>
       <c r="B98" s="55"/>
       <c r="C98" s="25" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="D98" s="50">
         <v>0</v>
@@ -8002,7 +8003,7 @@
         <v>182</v>
       </c>
       <c r="C101" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D101" s="50"/>
       <c r="E101" s="50">
@@ -8084,7 +8085,7 @@
         <v>185</v>
       </c>
       <c r="C103" s="25" t="s">
-        <v>628</v>
+        <v>617</v>
       </c>
       <c r="D103" s="50">
         <v>0</v>
@@ -8121,7 +8122,7 @@
       <c r="A104" s="54"/>
       <c r="B104" s="55"/>
       <c r="C104" s="25" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
       <c r="D104" s="50">
         <v>0</v>
@@ -8160,7 +8161,7 @@
       <c r="A105" s="54"/>
       <c r="B105" s="55"/>
       <c r="C105" s="25" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="D105" s="50">
         <v>0</v>
@@ -8306,7 +8307,7 @@
         <v>187</v>
       </c>
       <c r="C108" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D108" s="50"/>
       <c r="E108" s="50">
@@ -8695,7 +8696,7 @@
       <c r="A117" s="54"/>
       <c r="B117" s="55"/>
       <c r="C117" s="25" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="D117" s="50">
         <v>0</v>
@@ -8734,7 +8735,7 @@
       <c r="A118" s="54"/>
       <c r="B118" s="55"/>
       <c r="C118" s="25" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
       <c r="D118" s="50">
         <v>0</v>
@@ -8773,7 +8774,7 @@
       <c r="A119" s="54"/>
       <c r="B119" s="55"/>
       <c r="C119" s="25" t="s">
-        <v>628</v>
+        <v>617</v>
       </c>
       <c r="D119" s="50">
         <v>0</v>
@@ -9073,7 +9074,7 @@
         <v>209</v>
       </c>
       <c r="C126" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D126" s="50"/>
       <c r="E126" s="50">
@@ -9345,7 +9346,7 @@
         <v>218</v>
       </c>
       <c r="C132" s="64" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="D132" s="65">
         <v>0</v>
@@ -9660,8 +9661,8 @@
       <c r="E139" s="50">
         <v>1</v>
       </c>
-      <c r="F139" s="27" t="s">
-        <v>232</v>
+      <c r="F139" s="197" t="s">
+        <v>623</v>
       </c>
       <c r="G139" s="51">
         <v>0.3</v>
@@ -9691,7 +9692,7 @@
       <c r="A140" s="54"/>
       <c r="B140" s="55"/>
       <c r="C140" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D140" s="50">
         <v>1</v>
@@ -9699,8 +9700,8 @@
       <c r="E140" s="50">
         <v>1</v>
       </c>
-      <c r="F140" s="27" t="s">
-        <v>234</v>
+      <c r="F140" s="197" t="s">
+        <v>624</v>
       </c>
       <c r="G140" s="51">
         <v>0.2</v>
@@ -9730,7 +9731,7 @@
       <c r="A141" s="54"/>
       <c r="B141" s="55"/>
       <c r="C141" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D141" s="50">
         <v>1</v>
@@ -9738,8 +9739,8 @@
       <c r="E141" s="50">
         <v>1</v>
       </c>
-      <c r="F141" s="27" t="s">
-        <v>236</v>
+      <c r="F141" s="197" t="s">
+        <v>625</v>
       </c>
       <c r="G141" s="51">
         <v>0.1</v>
@@ -9769,7 +9770,7 @@
       <c r="A142" s="54"/>
       <c r="B142" s="55"/>
       <c r="C142" s="25" t="s">
-        <v>630</v>
+        <v>619</v>
       </c>
       <c r="D142" s="50">
         <v>0</v>
@@ -9808,7 +9809,7 @@
       <c r="A143" s="54"/>
       <c r="B143" s="55"/>
       <c r="C143" s="25" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="D143" s="50">
         <v>0</v>
@@ -9847,7 +9848,7 @@
       <c r="A144" s="54"/>
       <c r="B144" s="55"/>
       <c r="C144" s="25" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
       <c r="D144" s="50">
         <v>0</v>
@@ -9886,7 +9887,7 @@
       <c r="A145" s="54"/>
       <c r="B145" s="55"/>
       <c r="C145" s="25" t="s">
-        <v>632</v>
+        <v>621</v>
       </c>
       <c r="D145" s="50">
         <v>0</v>
@@ -9925,7 +9926,7 @@
       <c r="A146" s="54"/>
       <c r="B146" s="55"/>
       <c r="C146" s="25" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
       <c r="D146" s="50">
         <v>0</v>
@@ -10121,7 +10122,7 @@
         <v>25</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C151" s="13"/>
       <c r="D151" s="13"/>
@@ -10185,7 +10186,7 @@
     <row r="152" spans="1:27" ht="16">
       <c r="A152" s="48"/>
       <c r="B152" s="49" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C152" s="25" t="s">
         <v>221</v>
@@ -10196,8 +10197,8 @@
       <c r="E152" s="50">
         <v>1</v>
       </c>
-      <c r="F152" s="27" t="s">
-        <v>239</v>
+      <c r="F152" s="197" t="s">
+        <v>626</v>
       </c>
       <c r="G152" s="51">
         <v>0.5</v>
@@ -10238,8 +10239,8 @@
       <c r="E153" s="50">
         <v>1</v>
       </c>
-      <c r="F153" s="27" t="s">
-        <v>240</v>
+      <c r="F153" s="197" t="s">
+        <v>627</v>
       </c>
       <c r="G153" s="51">
         <v>0.3</v>
@@ -10268,7 +10269,7 @@
     <row r="154" spans="1:27" ht="16">
       <c r="A154" s="5"/>
       <c r="B154" s="63" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C154" s="25" t="s">
         <v>226</v>
@@ -10279,8 +10280,8 @@
       <c r="E154" s="50">
         <v>1</v>
       </c>
-      <c r="F154" s="27" t="s">
-        <v>242</v>
+      <c r="F154" s="197" t="s">
+        <v>628</v>
       </c>
       <c r="G154" s="51">
         <v>0.6</v>
@@ -10318,8 +10319,8 @@
       <c r="E155" s="50">
         <v>1</v>
       </c>
-      <c r="F155" s="27" t="s">
-        <v>243</v>
+      <c r="F155" s="197" t="s">
+        <v>629</v>
       </c>
       <c r="G155" s="51">
         <v>0.1</v>
@@ -10349,7 +10350,7 @@
       <c r="A156" s="54"/>
       <c r="B156" s="55"/>
       <c r="C156" s="81" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D156" s="50">
         <v>1</v>
@@ -10357,8 +10358,8 @@
       <c r="E156" s="50">
         <v>1</v>
       </c>
-      <c r="F156" s="27" t="s">
-        <v>245</v>
+      <c r="F156" s="197" t="s">
+        <v>630</v>
       </c>
       <c r="G156" s="51">
         <v>0.2</v>
@@ -10388,7 +10389,7 @@
       <c r="A157" s="54"/>
       <c r="B157" s="55"/>
       <c r="C157" s="81" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D157" s="50">
         <v>1</v>
@@ -10396,8 +10397,8 @@
       <c r="E157" s="50">
         <v>1</v>
       </c>
-      <c r="F157" s="27" t="s">
-        <v>247</v>
+      <c r="F157" s="197" t="s">
+        <v>631</v>
       </c>
       <c r="G157" s="51">
         <v>0.1</v>
@@ -10427,7 +10428,7 @@
       <c r="A158" s="54"/>
       <c r="B158" s="55"/>
       <c r="C158" s="81" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D158" s="50">
         <v>1</v>
@@ -10435,8 +10436,8 @@
       <c r="E158" s="50">
         <v>1</v>
       </c>
-      <c r="F158" s="27" t="s">
-        <v>249</v>
+      <c r="F158" s="197" t="s">
+        <v>632</v>
       </c>
       <c r="G158" s="51">
         <v>0.1</v>
@@ -10466,7 +10467,7 @@
       <c r="A159" s="54"/>
       <c r="B159" s="55"/>
       <c r="C159" s="81" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D159" s="50">
         <v>1</v>
@@ -10474,8 +10475,8 @@
       <c r="E159" s="50">
         <v>1</v>
       </c>
-      <c r="F159" s="27" t="s">
-        <v>251</v>
+      <c r="F159" s="197" t="s">
+        <v>633</v>
       </c>
       <c r="G159" s="51">
         <v>0.3</v>
@@ -10505,7 +10506,7 @@
       <c r="A160" s="54"/>
       <c r="B160" s="55"/>
       <c r="C160" s="25" t="s">
-        <v>630</v>
+        <v>619</v>
       </c>
       <c r="D160" s="50">
         <v>0</v>
@@ -10544,7 +10545,7 @@
       <c r="A161" s="54"/>
       <c r="B161" s="55"/>
       <c r="C161" s="25" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="D161" s="50">
         <v>0</v>
@@ -10583,7 +10584,7 @@
       <c r="A162" s="54"/>
       <c r="B162" s="55"/>
       <c r="C162" s="25" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
       <c r="D162" s="50">
         <v>0</v>
@@ -10622,7 +10623,7 @@
       <c r="A163" s="54"/>
       <c r="B163" s="55"/>
       <c r="C163" s="25" t="s">
-        <v>632</v>
+        <v>621</v>
       </c>
       <c r="D163" s="50">
         <v>0</v>
@@ -10661,7 +10662,7 @@
       <c r="A164" s="54"/>
       <c r="B164" s="57"/>
       <c r="C164" s="64" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
       <c r="D164" s="65">
         <v>0</v>
@@ -10701,7 +10702,7 @@
         <v>26</v>
       </c>
       <c r="B165" s="12" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C165" s="13"/>
       <c r="D165" s="13"/>
@@ -10765,10 +10766,10 @@
     <row r="166" spans="1:27" ht="16">
       <c r="A166" s="23"/>
       <c r="B166" s="24" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C166" s="25" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="D166" s="50"/>
       <c r="E166" s="50">
@@ -10809,7 +10810,7 @@
         <v>2.6</v>
       </c>
       <c r="C167" s="25" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="D167" s="25">
         <v>1</v>
@@ -10818,7 +10819,7 @@
         <v>1</v>
       </c>
       <c r="F167" s="84" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="G167" s="51">
         <v>0.4</v>
@@ -10847,10 +10848,10 @@
     <row r="168" spans="1:27" ht="16">
       <c r="A168" s="85"/>
       <c r="B168" s="86" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C168" s="25" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="D168" s="25">
         <v>1</v>
@@ -10859,7 +10860,7 @@
         <v>1</v>
       </c>
       <c r="F168" s="84" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="G168" s="51">
         <v>0</v>
@@ -10889,7 +10890,7 @@
       <c r="A169" s="11"/>
       <c r="B169" s="87"/>
       <c r="C169" s="25" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D169" s="25">
         <v>1</v>
@@ -10898,7 +10899,7 @@
         <v>7</v>
       </c>
       <c r="F169" s="84" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="G169" s="51">
         <v>0</v>
@@ -10928,7 +10929,7 @@
       <c r="A170" s="11"/>
       <c r="B170" s="88"/>
       <c r="C170" s="64" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D170" s="64">
         <v>1</v>
@@ -10937,7 +10938,7 @@
         <v>1</v>
       </c>
       <c r="F170" s="89" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="G170" s="67">
         <v>0</v>
@@ -10968,7 +10969,7 @@
         <v>27</v>
       </c>
       <c r="B171" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C171" s="90"/>
       <c r="D171" s="90"/>
@@ -11032,14 +11033,14 @@
     <row r="172" spans="1:27" ht="16">
       <c r="A172" s="34"/>
       <c r="C172" s="25" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="D172" s="50"/>
       <c r="E172" s="50">
         <v>1</v>
       </c>
       <c r="F172" s="56" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="G172" s="51">
         <v>40</v>
@@ -11048,7 +11049,7 @@
       <c r="I172" s="29"/>
       <c r="J172" s="30"/>
       <c r="K172" s="5" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="L172" s="29"/>
       <c r="M172" s="29"/>
@@ -11074,14 +11075,14 @@
         <v>187.8</v>
       </c>
       <c r="C173" s="25" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D173" s="50"/>
       <c r="E173" s="50">
         <v>1</v>
       </c>
       <c r="F173" s="56" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="G173" s="51">
         <v>64.5</v>
@@ -11111,14 +11112,14 @@
       <c r="A174" s="54"/>
       <c r="B174" s="55"/>
       <c r="C174" s="25" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D174" s="50"/>
       <c r="E174" s="50">
         <v>1</v>
       </c>
       <c r="F174" s="56" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="G174" s="51">
         <v>22.3</v>
@@ -11148,14 +11149,14 @@
       <c r="A175" s="54"/>
       <c r="B175" s="55"/>
       <c r="C175" s="25" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="D175" s="50"/>
       <c r="E175" s="50">
         <v>1</v>
       </c>
       <c r="F175" s="56" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="G175" s="51">
         <v>9.5</v>
@@ -11185,14 +11186,14 @@
       <c r="A176" s="54"/>
       <c r="B176" s="55"/>
       <c r="C176" s="25" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="D176" s="50"/>
       <c r="E176" s="50">
         <v>1</v>
       </c>
       <c r="F176" s="56" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="G176" s="51">
         <v>11</v>
@@ -11222,14 +11223,14 @@
       <c r="A177" s="54"/>
       <c r="B177" s="55"/>
       <c r="C177" s="25" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="D177" s="50"/>
       <c r="E177" s="50">
         <v>1</v>
       </c>
       <c r="F177" s="56" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="G177" s="51">
         <v>27</v>
@@ -11259,14 +11260,14 @@
       <c r="A178" s="54"/>
       <c r="B178" s="57"/>
       <c r="C178" s="64" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="D178" s="65"/>
       <c r="E178" s="65">
         <v>1</v>
       </c>
       <c r="F178" s="66" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G178" s="67">
         <v>13.5</v>
@@ -11297,7 +11298,7 @@
         <v>28</v>
       </c>
       <c r="B179" s="12" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C179" s="90"/>
       <c r="D179" s="90"/>
@@ -11328,7 +11329,7 @@
     <row r="180" spans="1:27" ht="16">
       <c r="A180" s="43"/>
       <c r="B180" s="93" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C180" s="94"/>
       <c r="D180" s="50"/>
@@ -11336,7 +11337,7 @@
         <v>1</v>
       </c>
       <c r="F180" s="56" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="G180" s="95">
         <v>7</v>
@@ -11395,7 +11396,7 @@
     <row r="181" spans="1:27" ht="16">
       <c r="A181" s="43"/>
       <c r="B181" s="93" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C181" s="94"/>
       <c r="D181" s="50"/>
@@ -11403,7 +11404,7 @@
         <v>1</v>
       </c>
       <c r="F181" s="56" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="G181" s="95">
         <v>13.1</v>
@@ -11462,7 +11463,7 @@
     <row r="182" spans="1:27" ht="16">
       <c r="A182" s="96"/>
       <c r="B182" s="97" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C182" s="94"/>
       <c r="D182" s="98"/>
@@ -11470,7 +11471,7 @@
         <v>1</v>
       </c>
       <c r="F182" s="27" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="G182" s="99">
         <v>0</v>
@@ -11529,7 +11530,7 @@
     <row r="183" spans="1:27" ht="16">
       <c r="A183" s="96"/>
       <c r="B183" s="97" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C183" s="94"/>
       <c r="D183" s="98"/>
@@ -11594,7 +11595,7 @@
     <row r="184" spans="1:27" ht="16">
       <c r="A184" s="96"/>
       <c r="B184" s="103" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C184" s="104"/>
       <c r="D184" s="105"/>
@@ -35709,18 +35710,18 @@
     <row r="1" spans="3:25" ht="15.75" customHeight="1"/>
     <row r="2" spans="3:25" ht="15.75" customHeight="1">
       <c r="C2" s="109" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="3:25" ht="15.75" customHeight="1"/>
     <row r="4" spans="3:25" ht="15.75" customHeight="1">
       <c r="C4" s="110" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="3:25" ht="15.75" customHeight="1">
       <c r="C5" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="3:25" ht="15.75" customHeight="1"/>
@@ -35728,28 +35729,28 @@
     <row r="8" spans="3:25" ht="15.75" customHeight="1"/>
     <row r="9" spans="3:25" ht="15.75" customHeight="1">
       <c r="C9" s="111" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="3:25" ht="15.75" customHeight="1">
       <c r="C10" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="3:25" ht="15.75" customHeight="1">
       <c r="C11" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="3:25" ht="15.75" customHeight="1">
       <c r="C12" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="3:25" ht="15.75" customHeight="1"/>
     <row r="14" spans="3:25" ht="15.75" customHeight="1">
       <c r="E14" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -35766,7 +35767,7 @@
     </row>
     <row r="15" spans="3:25" ht="15.75" customHeight="1">
       <c r="E15" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -35795,7 +35796,7 @@
     </row>
     <row r="16" spans="3:25" ht="15.75" customHeight="1">
       <c r="E16" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -35835,7 +35836,7 @@
     </row>
     <row r="17" spans="4:25" ht="15.75" customHeight="1">
       <c r="E17" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -35869,64 +35870,64 @@
         <v>56</v>
       </c>
       <c r="G18" s="114" t="s">
+        <v>288</v>
+      </c>
+      <c r="H18" s="115" t="s">
+        <v>289</v>
+      </c>
+      <c r="I18" s="115" t="s">
+        <v>290</v>
+      </c>
+      <c r="J18" s="115" t="s">
+        <v>291</v>
+      </c>
+      <c r="K18" s="115" t="s">
+        <v>292</v>
+      </c>
+      <c r="L18" s="115" t="s">
+        <v>293</v>
+      </c>
+      <c r="M18" s="115" t="s">
+        <v>294</v>
+      </c>
+      <c r="N18" s="115" t="s">
+        <v>295</v>
+      </c>
+      <c r="O18" s="115" t="s">
+        <v>296</v>
+      </c>
+      <c r="P18" s="115" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q18" s="115" t="s">
+        <v>298</v>
+      </c>
+      <c r="R18" s="115" t="s">
         <v>299</v>
       </c>
-      <c r="H18" s="115" t="s">
+      <c r="S18" s="115" t="s">
         <v>300</v>
       </c>
-      <c r="I18" s="115" t="s">
+      <c r="T18" s="115" t="s">
         <v>301</v>
       </c>
-      <c r="J18" s="115" t="s">
+      <c r="U18" s="115" t="s">
         <v>302</v>
       </c>
-      <c r="K18" s="115" t="s">
+      <c r="V18" s="115" t="s">
         <v>303</v>
       </c>
-      <c r="L18" s="115" t="s">
+      <c r="W18" s="115" t="s">
         <v>304</v>
       </c>
-      <c r="M18" s="115" t="s">
+      <c r="X18" s="112" t="s">
         <v>305</v>
-      </c>
-      <c r="N18" s="115" t="s">
-        <v>306</v>
-      </c>
-      <c r="O18" s="115" t="s">
-        <v>307</v>
-      </c>
-      <c r="P18" s="115" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q18" s="115" t="s">
-        <v>309</v>
-      </c>
-      <c r="R18" s="115" t="s">
-        <v>310</v>
-      </c>
-      <c r="S18" s="115" t="s">
-        <v>311</v>
-      </c>
-      <c r="T18" s="115" t="s">
-        <v>312</v>
-      </c>
-      <c r="U18" s="115" t="s">
-        <v>313</v>
-      </c>
-      <c r="V18" s="115" t="s">
-        <v>314</v>
-      </c>
-      <c r="W18" s="115" t="s">
-        <v>315</v>
-      </c>
-      <c r="X18" s="112" t="s">
-        <v>316</v>
       </c>
       <c r="Y18" s="112"/>
     </row>
     <row r="19" spans="4:25" ht="15.75" customHeight="1">
       <c r="E19" s="116" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="F19" s="117"/>
       <c r="G19" s="117"/>
@@ -35952,11 +35953,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="118" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="F20" s="117"/>
       <c r="G20" s="117" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="H20" s="117">
         <v>1</v>
@@ -35994,11 +35995,11 @@
         <v>2</v>
       </c>
       <c r="E21" s="118" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="F21" s="117"/>
       <c r="G21" s="117" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="H21" s="117"/>
       <c r="I21" s="117">
@@ -36024,11 +36025,11 @@
         <v>3</v>
       </c>
       <c r="E22" s="118" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F22" s="117"/>
       <c r="G22" s="117" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="H22" s="117"/>
       <c r="I22" s="117"/>
@@ -36066,11 +36067,11 @@
         <v>4</v>
       </c>
       <c r="E23" s="118" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="F23" s="117"/>
       <c r="G23" s="117" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="H23" s="117"/>
       <c r="I23" s="117"/>
@@ -36106,11 +36107,11 @@
         <v>5</v>
       </c>
       <c r="E24" s="118" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="F24" s="117"/>
       <c r="G24" s="117" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="H24" s="117"/>
       <c r="I24" s="117"/>
@@ -36133,7 +36134,7 @@
       <c r="V24" s="117"/>
       <c r="W24" s="117"/>
       <c r="X24" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="4:25" ht="15.75" customHeight="1">
@@ -36141,11 +36142,11 @@
         <v>6</v>
       </c>
       <c r="E25" s="118" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="F25" s="117"/>
       <c r="G25" s="117" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="H25" s="117"/>
       <c r="I25" s="117">
@@ -36171,11 +36172,11 @@
         <v>7</v>
       </c>
       <c r="E26" s="118" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="F26" s="117"/>
       <c r="G26" s="117" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="H26" s="117"/>
       <c r="I26" s="117">
@@ -36204,7 +36205,7 @@
       <c r="V26" s="117"/>
       <c r="W26" s="117"/>
       <c r="X26" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="4:25" ht="15.75" customHeight="1">
@@ -36216,7 +36217,7 @@
       </c>
       <c r="F27" s="117"/>
       <c r="G27" s="117" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="H27" s="117"/>
       <c r="I27" s="117">
@@ -36243,7 +36244,7 @@
         <v>1</v>
       </c>
       <c r="X27" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="4:25" ht="15.75" customHeight="1">
@@ -36251,11 +36252,11 @@
         <v>9</v>
       </c>
       <c r="E28" s="118" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="F28" s="117"/>
       <c r="G28" s="117" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="H28" s="117">
         <v>1</v>
@@ -36285,7 +36286,7 @@
         <v>10</v>
       </c>
       <c r="E29" s="119" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="F29" s="117"/>
       <c r="G29" s="117"/>
@@ -37367,7 +37368,7 @@
   <sheetData>
     <row r="1" spans="2:57" ht="15.75" customHeight="1">
       <c r="B1" s="48" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="AD1" s="48"/>
       <c r="AE1" s="48"/>
@@ -37384,14 +37385,14 @@
       <c r="AN1" s="48"/>
       <c r="AO1" s="48"/>
       <c r="AP1" s="48" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="AQ1" s="48" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="AR1" s="48"/>
       <c r="AS1" s="48" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="AT1" s="48"/>
       <c r="AU1" s="48"/>
@@ -37403,101 +37404,101 @@
       <c r="BA1" s="48"/>
       <c r="BB1" s="48"/>
       <c r="BC1" s="48" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="BD1" s="48" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="2:57" ht="15.75" customHeight="1">
       <c r="B2" s="48" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="AD2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AE2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AF2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AG2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AH2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AI2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AJ2" s="48" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="AK2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AL2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AM2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AN2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AO2" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AP2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AQ2" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AR2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AS2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AT2" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AU2" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AV2" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AW2" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AX2" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AY2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="AZ2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="BA2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="BB2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="BC2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="BD2" s="48" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="2:57" ht="15.75" customHeight="1">
       <c r="B3" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -37689,67 +37690,67 @@
       <c r="AB4" s="120"/>
       <c r="AC4" s="120"/>
       <c r="AD4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AE4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AF4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AG4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AH4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AI4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AJ4" s="48" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="AK4" s="123" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="AL4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AM4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AN4" s="48" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="AO4" s="48" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="AP4" s="48" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="AQ4" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AR4" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="AS4" s="48" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="AT4" s="48" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="AU4" s="48" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="AV4" s="48" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="AW4" s="48" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="AX4" s="48" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="AY4" s="48"/>
       <c r="AZ4" s="48"/>
@@ -37760,7 +37761,7 @@
     </row>
     <row r="5" spans="2:57" ht="15.75" customHeight="1">
       <c r="B5" s="120" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="C5" s="120"/>
       <c r="D5" s="121"/>
@@ -37793,10 +37794,10 @@
         <v>140</v>
       </c>
       <c r="AE5" s="69" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="AF5" s="127" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="AG5" s="69" t="s">
         <v>180</v>
@@ -37811,7 +37812,7 @@
         <v>126</v>
       </c>
       <c r="AK5" s="123" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="AL5" s="69" t="s">
         <v>109</v>
@@ -37820,22 +37821,22 @@
         <v>111</v>
       </c>
       <c r="AN5" s="69" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="AO5" s="69" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="AP5" s="69" t="s">
         <v>101</v>
       </c>
       <c r="AQ5" s="69" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="AR5" s="69" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="AS5" s="69" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="AT5" s="69" t="s">
         <v>74</v>
@@ -37847,10 +37848,10 @@
         <v>141</v>
       </c>
       <c r="AW5" s="69" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="AX5" s="69" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="AY5" s="69" t="s">
         <v>108</v>
@@ -37859,164 +37860,164 @@
         <v>108</v>
       </c>
       <c r="BA5" s="69" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="BB5" s="69" t="s">
         <v>93</v>
       </c>
       <c r="BC5" s="124" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="BD5" s="124" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="2:57" ht="15.75" customHeight="1">
       <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" t="s">
+        <v>351</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>352</v>
+      </c>
+      <c r="AE6" s="48" t="s">
+        <v>353</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>354</v>
+      </c>
+      <c r="AG6" s="129" t="s">
+        <v>355</v>
+      </c>
+      <c r="AH6" s="130" t="s">
+        <v>356</v>
+      </c>
+      <c r="AI6" s="130" t="s">
+        <v>357</v>
+      </c>
+      <c r="AJ6" s="130" t="s">
+        <v>358</v>
+      </c>
+      <c r="AK6" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>360</v>
+      </c>
+      <c r="AM6" s="48" t="s">
         <v>361</v>
       </c>
-      <c r="D6" t="s">
+      <c r="AN6" s="48" t="s">
         <v>362</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AO6" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="AE6" s="48" t="s">
+      <c r="AP6" t="s">
         <v>364</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AQ6" t="s">
         <v>365</v>
       </c>
-      <c r="AG6" s="129" t="s">
+      <c r="AR6" s="129" t="s">
         <v>366</v>
       </c>
-      <c r="AH6" s="130" t="s">
+      <c r="AS6" t="s">
         <v>367</v>
       </c>
-      <c r="AI6" s="130" t="s">
+      <c r="AT6" s="48" t="s">
         <v>368</v>
       </c>
-      <c r="AJ6" s="130" t="s">
+      <c r="AU6" s="48" t="s">
         <v>369</v>
       </c>
-      <c r="AK6" s="48" t="s">
+      <c r="AV6" s="48" t="s">
         <v>370</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AW6" s="48" t="s">
         <v>371</v>
       </c>
-      <c r="AM6" s="48" t="s">
+      <c r="AX6" s="48" t="s">
+        <v>371</v>
+      </c>
+      <c r="AY6" s="48" t="s">
         <v>372</v>
       </c>
-      <c r="AN6" s="48" t="s">
+      <c r="AZ6" s="48" t="s">
+        <v>372</v>
+      </c>
+      <c r="BA6" s="48" t="s">
         <v>373</v>
       </c>
-      <c r="AO6" s="48" t="s">
+      <c r="BB6" s="48" t="s">
         <v>374</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="BC6" s="48" t="s">
         <v>375</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="BD6" s="48" t="s">
         <v>376</v>
-      </c>
-      <c r="AR6" s="129" t="s">
-        <v>377</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>378</v>
-      </c>
-      <c r="AT6" s="48" t="s">
-        <v>379</v>
-      </c>
-      <c r="AU6" s="48" t="s">
-        <v>380</v>
-      </c>
-      <c r="AV6" s="48" t="s">
-        <v>381</v>
-      </c>
-      <c r="AW6" s="48" t="s">
-        <v>382</v>
-      </c>
-      <c r="AX6" s="48" t="s">
-        <v>382</v>
-      </c>
-      <c r="AY6" s="48" t="s">
-        <v>383</v>
-      </c>
-      <c r="AZ6" s="48" t="s">
-        <v>383</v>
-      </c>
-      <c r="BA6" s="48" t="s">
-        <v>384</v>
-      </c>
-      <c r="BB6" s="48" t="s">
-        <v>385</v>
-      </c>
-      <c r="BC6" s="48" t="s">
-        <v>386</v>
-      </c>
-      <c r="BD6" s="48" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="7" spans="2:57" ht="15.75" customHeight="1">
       <c r="B7" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="D7" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="E7" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="F7" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="G7" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="H7" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="I7" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="J7" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="K7" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="L7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="M7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="N7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="O7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="P7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="Q7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="R7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="S7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="T7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="U7" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="2:57" ht="15.75" hidden="1" customHeight="1"/>
@@ -38026,7 +38027,7 @@
     <row r="12" spans="2:57" ht="15.75" hidden="1" customHeight="1"/>
     <row r="13" spans="2:57" ht="15.75" customHeight="1">
       <c r="B13" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="D13" s="131">
         <v>4</v>
@@ -38243,7 +38244,7 @@
     </row>
     <row r="14" spans="2:57" ht="15.75" customHeight="1">
       <c r="B14" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D14" s="132">
         <f t="shared" ref="D14:AC14" si="2">D13*D3</f>
@@ -38460,7 +38461,7 @@
     </row>
     <row r="15" spans="2:57" ht="15.75" customHeight="1">
       <c r="B15" s="48" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="D15" s="132"/>
       <c r="E15" s="132"/>
@@ -38519,174 +38520,174 @@
     </row>
     <row r="16" spans="2:57" ht="150" customHeight="1">
       <c r="B16" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="C16" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="114" t="s">
+        <v>384</v>
+      </c>
+      <c r="E16" s="115" t="s">
+        <v>385</v>
+      </c>
+      <c r="F16" s="115" t="s">
+        <v>386</v>
+      </c>
+      <c r="G16" s="115" t="s">
+        <v>387</v>
+      </c>
+      <c r="H16" s="115" t="s">
+        <v>388</v>
+      </c>
+      <c r="I16" s="115" t="s">
+        <v>389</v>
+      </c>
+      <c r="J16" s="115" t="s">
+        <v>390</v>
+      </c>
+      <c r="K16" s="115" t="s">
+        <v>391</v>
+      </c>
+      <c r="L16" s="134" t="s">
+        <v>392</v>
+      </c>
+      <c r="M16" s="134" t="s">
+        <v>393</v>
+      </c>
+      <c r="N16" s="134" t="s">
+        <v>394</v>
+      </c>
+      <c r="O16" s="134" t="s">
         <v>395</v>
       </c>
-      <c r="E16" s="115" t="s">
+      <c r="P16" s="134" t="s">
         <v>396</v>
       </c>
-      <c r="F16" s="115" t="s">
+      <c r="Q16" s="134" t="s">
         <v>397</v>
       </c>
-      <c r="G16" s="115" t="s">
+      <c r="R16" s="134" t="s">
         <v>398</v>
       </c>
-      <c r="H16" s="115" t="s">
+      <c r="S16" s="134" t="s">
         <v>399</v>
       </c>
-      <c r="I16" s="115" t="s">
+      <c r="T16" s="134" t="s">
         <v>400</v>
       </c>
-      <c r="J16" s="115" t="s">
+      <c r="U16" s="134" t="s">
         <v>401</v>
       </c>
-      <c r="K16" s="115" t="s">
+      <c r="V16" s="134" t="s">
         <v>402</v>
       </c>
-      <c r="L16" s="134" t="s">
+      <c r="W16" s="135" t="s">
         <v>403</v>
       </c>
-      <c r="M16" s="134" t="s">
+      <c r="X16" s="135" t="s">
         <v>404</v>
       </c>
-      <c r="N16" s="134" t="s">
+      <c r="Y16" s="135" t="s">
         <v>405</v>
       </c>
-      <c r="O16" s="134" t="s">
+      <c r="Z16" s="135" t="s">
         <v>406</v>
       </c>
-      <c r="P16" s="134" t="s">
+      <c r="AA16" s="135" t="s">
         <v>407</v>
       </c>
-      <c r="Q16" s="134" t="s">
+      <c r="AB16" s="135" t="s">
         <v>408</v>
       </c>
-      <c r="R16" s="134" t="s">
+      <c r="AC16" s="135" t="s">
         <v>409</v>
       </c>
-      <c r="S16" s="134" t="s">
+      <c r="AD16" s="136" t="s">
         <v>410</v>
       </c>
-      <c r="T16" s="134" t="s">
+      <c r="AE16" s="136" t="s">
         <v>411</v>
       </c>
-      <c r="U16" s="134" t="s">
+      <c r="AF16" s="136" t="s">
         <v>412</v>
       </c>
-      <c r="V16" s="134" t="s">
+      <c r="AG16" s="136" t="s">
         <v>413</v>
       </c>
-      <c r="W16" s="135" t="s">
+      <c r="AH16" s="136" t="s">
         <v>414</v>
       </c>
-      <c r="X16" s="135" t="s">
+      <c r="AI16" s="137" t="s">
         <v>415</v>
       </c>
-      <c r="Y16" s="135" t="s">
+      <c r="AJ16" s="136" t="s">
         <v>416</v>
       </c>
-      <c r="Z16" s="135" t="s">
+      <c r="AK16" s="136" t="s">
         <v>417</v>
       </c>
-      <c r="AA16" s="135" t="s">
+      <c r="AL16" s="136" t="s">
         <v>418</v>
       </c>
-      <c r="AB16" s="135" t="s">
+      <c r="AM16" s="136" t="s">
         <v>419</v>
       </c>
-      <c r="AC16" s="135" t="s">
+      <c r="AN16" s="137" t="s">
         <v>420</v>
       </c>
-      <c r="AD16" s="136" t="s">
+      <c r="AO16" s="136" t="s">
         <v>421</v>
       </c>
-      <c r="AE16" s="136" t="s">
+      <c r="AP16" s="136" t="s">
         <v>422</v>
       </c>
-      <c r="AF16" s="136" t="s">
+      <c r="AQ16" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="AG16" s="136" t="s">
+      <c r="AR16" s="136" t="s">
         <v>424</v>
       </c>
-      <c r="AH16" s="136" t="s">
+      <c r="AS16" s="136" t="s">
         <v>425</v>
       </c>
-      <c r="AI16" s="137" t="s">
+      <c r="AT16" s="137" t="s">
         <v>426</v>
       </c>
-      <c r="AJ16" s="136" t="s">
+      <c r="AU16" s="137" t="s">
         <v>427</v>
       </c>
-      <c r="AK16" s="136" t="s">
+      <c r="AV16" s="137" t="s">
         <v>428</v>
       </c>
-      <c r="AL16" s="136" t="s">
+      <c r="AW16" s="137" t="s">
         <v>429</v>
       </c>
-      <c r="AM16" s="136" t="s">
+      <c r="AX16" s="137" t="s">
         <v>430</v>
       </c>
-      <c r="AN16" s="137" t="s">
+      <c r="AY16" s="136" t="s">
         <v>431</v>
       </c>
-      <c r="AO16" s="136" t="s">
+      <c r="AZ16" s="136" t="s">
         <v>432</v>
       </c>
-      <c r="AP16" s="136" t="s">
+      <c r="BA16" s="136" t="s">
         <v>433</v>
       </c>
-      <c r="AQ16" s="136" t="s">
+      <c r="BB16" s="136" t="s">
         <v>434</v>
       </c>
-      <c r="AR16" s="136" t="s">
+      <c r="BC16" s="137" t="s">
         <v>435</v>
       </c>
-      <c r="AS16" s="136" t="s">
+      <c r="BD16" s="137" t="s">
         <v>436</v>
-      </c>
-      <c r="AT16" s="137" t="s">
-        <v>437</v>
-      </c>
-      <c r="AU16" s="137" t="s">
-        <v>438</v>
-      </c>
-      <c r="AV16" s="137" t="s">
-        <v>439</v>
-      </c>
-      <c r="AW16" s="137" t="s">
-        <v>440</v>
-      </c>
-      <c r="AX16" s="137" t="s">
-        <v>441</v>
-      </c>
-      <c r="AY16" s="136" t="s">
-        <v>442</v>
-      </c>
-      <c r="AZ16" s="136" t="s">
-        <v>443</v>
-      </c>
-      <c r="BA16" s="136" t="s">
-        <v>444</v>
-      </c>
-      <c r="BB16" s="136" t="s">
-        <v>445</v>
-      </c>
-      <c r="BC16" s="137" t="s">
-        <v>446</v>
-      </c>
-      <c r="BD16" s="137" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="17" spans="2:56" ht="15.75" customHeight="1">
       <c r="B17" s="138" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -38726,7 +38727,7 @@
     </row>
     <row r="19" spans="2:56" ht="15.75" customHeight="1">
       <c r="B19" s="139" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -38784,7 +38785,7 @@
     </row>
     <row r="21" spans="2:56" ht="15.75" customHeight="1">
       <c r="B21" s="139" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -38837,7 +38838,7 @@
     </row>
     <row r="22" spans="2:56" ht="15.75" customHeight="1">
       <c r="B22" s="139" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -38875,7 +38876,7 @@
     </row>
     <row r="23" spans="2:56" ht="15.75" customHeight="1">
       <c r="B23" s="139" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -38910,7 +38911,7 @@
     </row>
     <row r="24" spans="2:56" ht="15.75" customHeight="1">
       <c r="B24" s="139" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -38977,7 +38978,7 @@
     </row>
     <row r="26" spans="2:56" ht="15.75" customHeight="1">
       <c r="B26" s="139" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -39009,7 +39010,7 @@
     </row>
     <row r="27" spans="2:56" ht="15.75" customHeight="1">
       <c r="B27" s="139" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -39035,7 +39036,7 @@
     </row>
     <row r="28" spans="2:56" ht="15.75" customHeight="1">
       <c r="B28" s="139" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -39058,7 +39059,7 @@
     </row>
     <row r="29" spans="2:56" ht="15.75" customHeight="1">
       <c r="B29" s="139" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -39095,7 +39096,7 @@
     </row>
     <row r="31" spans="2:56" ht="15.75" customHeight="1">
       <c r="B31" s="139" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -39112,7 +39113,7 @@
     </row>
     <row r="32" spans="2:56" ht="15.75" customHeight="1">
       <c r="B32" s="139" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -39135,7 +39136,7 @@
     </row>
     <row r="33" spans="2:50" ht="15.75" customHeight="1">
       <c r="B33" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -39172,7 +39173,7 @@
     <row r="35" spans="2:50" ht="15.75" customHeight="1"/>
     <row r="36" spans="2:50" ht="15.75" customHeight="1">
       <c r="B36" s="139" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="C36">
         <f>SUM(C17:C35)</f>
@@ -39182,33 +39183,33 @@
     <row r="37" spans="2:50" ht="15.75" customHeight="1"/>
     <row r="38" spans="2:50" ht="15.75" customHeight="1">
       <c r="B38" s="140" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="D38" s="48" t="s">
         <v>55</v>
       </c>
       <c r="E38" s="48" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="F38" s="48" t="s">
         <v>60</v>
       </c>
       <c r="G38" s="48" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="H38" s="48" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="I38" s="48" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
     </row>
     <row r="39" spans="2:50" ht="15.75" customHeight="1">
       <c r="B39" s="130" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="C39" s="48">
         <v>4.8899999999999997</v>
@@ -39224,12 +39225,12 @@
         <v>93</v>
       </c>
       <c r="G39" s="48" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
     <row r="40" spans="2:50" ht="15.75" customHeight="1">
       <c r="B40" s="48" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="C40" s="48">
         <v>4.8899999999999997</v>
@@ -39245,12 +39246,12 @@
         <v>93</v>
       </c>
       <c r="G40" s="48" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
     <row r="41" spans="2:50" ht="15.75" customHeight="1">
       <c r="B41" s="48" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="C41" s="48">
         <v>55</v>
@@ -39263,15 +39264,15 @@
         <v>55</v>
       </c>
       <c r="F41" s="69" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="G41" s="48" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
     </row>
     <row r="42" spans="2:50" ht="15.75" customHeight="1">
       <c r="B42" s="48" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="C42" s="48">
         <v>4.8899999999999997</v>
@@ -39287,12 +39288,12 @@
         <v>93</v>
       </c>
       <c r="G42" s="48" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
     </row>
     <row r="43" spans="2:50" ht="15.75" customHeight="1">
       <c r="B43" s="48" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="C43" s="48">
         <v>1.6</v>
@@ -39305,21 +39306,21 @@
         <v>1.6</v>
       </c>
       <c r="F43" s="69" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
       <c r="G43" s="48" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="I43" s="69" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
       <c r="J43" s="48" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
     </row>
     <row r="44" spans="2:50" ht="15.75" customHeight="1">
       <c r="B44" s="48" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="C44" s="48">
         <v>1.6</v>
@@ -39332,15 +39333,15 @@
         <v>1.6</v>
       </c>
       <c r="F44" s="69" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
       <c r="G44" s="48" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="2:50" ht="15.75" customHeight="1">
       <c r="B45" s="140" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="E45">
         <f t="shared" si="4"/>
@@ -39349,7 +39350,7 @@
     </row>
     <row r="46" spans="2:50" ht="15.75" customHeight="1">
       <c r="B46" s="48" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
       <c r="C46" s="48">
         <v>39</v>
@@ -39362,15 +39363,15 @@
         <v>39</v>
       </c>
       <c r="F46" s="69" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
       <c r="G46" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="47" spans="2:50" ht="15.75" customHeight="1">
       <c r="B47" s="48" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="C47" s="48">
         <v>10</v>
@@ -39383,15 +39384,15 @@
         <v>10</v>
       </c>
       <c r="F47" s="69" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
       <c r="G47" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="2:50" ht="15.75" customHeight="1">
       <c r="B48" s="48" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="C48" s="48">
         <v>11</v>
@@ -39404,15 +39405,15 @@
         <v>11</v>
       </c>
       <c r="F48" s="69" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="G48" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="15.75" customHeight="1">
       <c r="B49" s="48" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="C49" s="48">
         <v>15</v>
@@ -39425,10 +39426,10 @@
         <v>15</v>
       </c>
       <c r="F49" s="69" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="G49" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="50" spans="2:9" ht="15.75" customHeight="1">
@@ -39439,7 +39440,7 @@
     </row>
     <row r="51" spans="2:9" ht="15.75" customHeight="1">
       <c r="B51" s="141" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="E51">
         <f t="shared" si="4"/>
@@ -39448,7 +39449,7 @@
     </row>
     <row r="52" spans="2:9" ht="15.75" customHeight="1">
       <c r="B52" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="C52" s="48">
         <v>11</v>
@@ -39461,15 +39462,15 @@
         <v>11</v>
       </c>
       <c r="F52" s="69" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="G52" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="53" spans="2:9" ht="15.75" customHeight="1">
       <c r="B53" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="C53" s="48">
         <v>5.99</v>
@@ -39482,15 +39483,15 @@
         <v>5.99</v>
       </c>
       <c r="F53" s="69" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="G53" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="54" spans="2:9" ht="15.75" customHeight="1">
       <c r="B54" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="C54" s="48">
         <v>2</v>
@@ -39503,15 +39504,15 @@
         <v>2</v>
       </c>
       <c r="F54" s="69" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="G54" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="55" spans="2:9" ht="15.75" customHeight="1">
       <c r="B55" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="C55" s="48">
         <v>15</v>
@@ -39527,12 +39528,12 @@
         <v>131</v>
       </c>
       <c r="G55" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="56" spans="2:9" ht="15.75" customHeight="1">
       <c r="B56" s="48" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="C56" s="48">
         <v>12</v>
@@ -39548,12 +39549,12 @@
         <v>128</v>
       </c>
       <c r="G56" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="57" spans="2:9" ht="15.75" customHeight="1">
       <c r="B57" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C57">
         <v>5</v>
@@ -39566,12 +39567,12 @@
         <v>5</v>
       </c>
       <c r="F57" s="48" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
     </row>
     <row r="58" spans="2:9" ht="15.75" customHeight="1">
       <c r="B58" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
       <c r="C58">
         <v>5</v>
@@ -39584,12 +39585,12 @@
         <v>5</v>
       </c>
       <c r="F58" s="48" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="15.75" customHeight="1">
       <c r="B59" s="48" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="C59" s="48">
         <v>10</v>
@@ -39602,12 +39603,12 @@
         <v>10</v>
       </c>
       <c r="F59" s="69" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
     </row>
     <row r="60" spans="2:9" ht="16">
       <c r="B60" s="48" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="C60" s="48">
         <v>1.8</v>
@@ -39620,21 +39621,21 @@
         <v>1.8</v>
       </c>
       <c r="F60" s="69" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="G60" s="48" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="H60" s="48" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="I60" s="48" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
     </row>
     <row r="61" spans="2:9" ht="15.75" customHeight="1">
       <c r="B61" s="48" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="C61" s="48">
         <v>0.36</v>
@@ -39647,21 +39648,21 @@
         <v>0.36</v>
       </c>
       <c r="F61" s="69" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="G61" s="48" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="H61" s="48" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="I61" s="48" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
     </row>
     <row r="62" spans="2:9" ht="15.75" customHeight="1">
       <c r="B62" s="48" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="D62" s="48">
         <v>1</v>
@@ -39673,7 +39674,7 @@
     </row>
     <row r="63" spans="2:9" ht="15.75" customHeight="1">
       <c r="B63" s="48" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="C63" s="48">
         <v>20</v>
@@ -39686,10 +39687,10 @@
         <v>20</v>
       </c>
       <c r="F63" s="69" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="G63" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="64" spans="2:9" ht="15.75" customHeight="1">
@@ -39700,7 +39701,7 @@
     </row>
     <row r="65" spans="2:7" ht="15.75" customHeight="1">
       <c r="B65" s="140" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="E65">
         <f t="shared" si="4"/>
@@ -39709,7 +39710,7 @@
     </row>
     <row r="66" spans="2:7" ht="15.75" customHeight="1">
       <c r="B66" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="C66" s="48">
         <v>45</v>
@@ -39722,15 +39723,15 @@
         <v>45</v>
       </c>
       <c r="F66" s="69" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="G66" s="48" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
     </row>
     <row r="67" spans="2:7" ht="15.75" customHeight="1">
       <c r="B67" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="C67" s="48">
         <v>9</v>
@@ -39743,15 +39744,15 @@
         <v>9</v>
       </c>
       <c r="F67" s="69" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="G67" s="48" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
     </row>
     <row r="68" spans="2:7" ht="15.75" customHeight="1">
       <c r="B68" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="C68">
         <v>70</v>
@@ -39764,15 +39765,15 @@
         <v>70</v>
       </c>
       <c r="F68" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="G68" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="15.75" customHeight="1">
       <c r="B69" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="C69" s="48">
         <v>15</v>
@@ -39785,15 +39786,15 @@
         <v>15</v>
       </c>
       <c r="F69" s="69" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="G69" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="70" spans="2:7" ht="15.75" customHeight="1">
       <c r="B70" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
       <c r="C70" s="48">
         <v>12</v>
@@ -39806,15 +39807,15 @@
         <v>12</v>
       </c>
       <c r="F70" s="69" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="G70" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="2:7" ht="15.75" customHeight="1">
       <c r="B71" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C71" s="48">
         <v>25</v>
@@ -39827,15 +39828,15 @@
         <v>25</v>
       </c>
       <c r="F71" s="69" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="G71" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="72" spans="2:7" ht="15.75" customHeight="1">
       <c r="B72" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="C72" s="48">
         <v>3</v>
@@ -39848,30 +39849,30 @@
         <v>3</v>
       </c>
       <c r="F72" s="69" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
       <c r="G72" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="73" spans="2:7" ht="15.75" customHeight="1">
       <c r="B73" s="48" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
       <c r="E73">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F73" s="48" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="G73" s="48" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
     </row>
     <row r="74" spans="2:7" ht="15.75" customHeight="1">
       <c r="B74" s="48" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="C74" s="48">
         <v>8.99</v>
@@ -39884,17 +39885,17 @@
         <v>8.99</v>
       </c>
       <c r="F74" s="69" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="G74" s="48" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="75" spans="2:7" ht="15.75" customHeight="1"/>
     <row r="76" spans="2:7" ht="15.75" customHeight="1"/>
     <row r="77" spans="2:7" ht="15.75" customHeight="1">
       <c r="B77" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="E77">
         <f>SUM(E39:E72)</f>
@@ -39904,14 +39905,14 @@
     <row r="78" spans="2:7" ht="15.75" customHeight="1"/>
     <row r="79" spans="2:7" ht="15.75" customHeight="1">
       <c r="B79" s="142" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C79" s="143">
         <f>E77+BE14</f>
         <v>735.58200000000011</v>
       </c>
       <c r="D79" s="142" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
     </row>
     <row r="80" spans="2:7" ht="15.75" customHeight="1"/>
@@ -39931,7 +39932,7 @@
     <row r="94" spans="2:55" ht="15.75" customHeight="1"/>
     <row r="95" spans="2:55" ht="15.75" customHeight="1">
       <c r="B95" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
     </row>
     <row r="96" spans="2:55" ht="15.75" customHeight="1">
@@ -44427,28 +44428,28 @@
     <row r="1" spans="1:26">
       <c r="A1" s="144"/>
       <c r="B1" s="145" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="C1" s="144" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="D1" s="146" t="s">
         <v>59</v>
       </c>
       <c r="E1" s="146" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
       <c r="F1" s="146" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
       <c r="G1" s="146" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="H1" s="146" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="I1" s="146" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="J1" s="147"/>
       <c r="K1" s="147"/>
@@ -44470,23 +44471,23 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="150" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
       <c r="B2" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C2" s="147"/>
       <c r="D2" s="147"/>
       <c r="E2" s="147"/>
       <c r="F2" s="147" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="G2" s="152" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="H2" s="147"/>
       <c r="I2" s="153" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="J2" s="147"/>
       <c r="K2" s="147"/>
@@ -44508,10 +44509,10 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="154" t="s">
-        <v>539</v>
+        <v>528</v>
       </c>
       <c r="B3" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C3" s="155">
         <v>65.81</v>
@@ -44523,13 +44524,13 @@
         <v>101</v>
       </c>
       <c r="F3" s="147" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="G3" s="157" t="s">
-        <v>540</v>
+        <v>529</v>
       </c>
       <c r="H3" s="158" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="I3" s="148"/>
       <c r="J3" s="147"/>
@@ -44552,10 +44553,10 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="150" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="B4" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C4" s="155">
         <v>34.840000000000003</v>
@@ -44568,13 +44569,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="F4" s="147" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="G4" s="152" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="H4" s="158" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="I4" s="148"/>
       <c r="J4" s="147"/>
@@ -44597,13 +44598,13 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="150" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="B5" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C5" s="160" t="s">
-        <v>543</v>
+        <v>532</v>
       </c>
       <c r="D5" s="156">
         <v>2</v>
@@ -44613,13 +44614,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="F5" s="147" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="G5" s="152" t="s">
-        <v>544</v>
+        <v>533</v>
       </c>
       <c r="H5" s="158" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="I5" s="148"/>
       <c r="J5" s="147"/>
@@ -44642,10 +44643,10 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="161" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="B6" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C6" s="147"/>
       <c r="D6" s="156">
@@ -44656,14 +44657,14 @@
         <v>#VALUE!</v>
       </c>
       <c r="F6" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G6" s="163" t="s">
         <v>174</v>
       </c>
       <c r="H6" s="148"/>
       <c r="I6" s="164" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="J6" s="147"/>
       <c r="K6" s="147"/>
@@ -44685,25 +44686,25 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="161" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="B7" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C7" s="147"/>
       <c r="D7" s="147">
         <v>1</v>
       </c>
       <c r="E7" s="152" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="F7" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G7" s="147"/>
       <c r="H7" s="147"/>
       <c r="I7" s="147" t="s">
-        <v>547</v>
+        <v>536</v>
       </c>
       <c r="J7" s="147"/>
       <c r="K7" s="147"/>
@@ -44725,10 +44726,10 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="161" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="B8" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C8" s="147"/>
       <c r="D8" s="147">
@@ -44738,7 +44739,7 @@
         <v>128</v>
       </c>
       <c r="F8" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G8" s="147"/>
       <c r="H8" s="147"/>
@@ -44763,10 +44764,10 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="161" t="s">
-        <v>548</v>
+        <v>537</v>
       </c>
       <c r="B9" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C9" s="147"/>
       <c r="D9" s="156">
@@ -44777,7 +44778,7 @@
         <v>https://www.amazon.de/Edelstahl-Sechskopf-Knopf-Schrauben-Unterlegscheiben-Sortiment-Aufbewahrung/dp/B073SS7D8J/ref=sr_1_fkmr0_1?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=zylinderkopfschrauben+set+galvanisiert&amp;qid=1565007371&amp;s=diy&amp;sr=1-1-fkmr0</v>
       </c>
       <c r="F9" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G9" s="147"/>
       <c r="H9" s="147"/>
@@ -44802,7 +44803,7 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="165" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="B10" s="166"/>
       <c r="C10" s="147"/>
@@ -44810,10 +44811,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="152" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="F10" s="147" t="s">
-        <v>549</v>
+        <v>538</v>
       </c>
       <c r="G10" s="147"/>
       <c r="H10" s="167"/>
@@ -44838,10 +44839,10 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="150" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="B11" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C11" s="160">
         <v>19.95</v>
@@ -44850,15 +44851,15 @@
         <v>1</v>
       </c>
       <c r="E11" s="152" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="F11" s="169" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="G11" s="147"/>
       <c r="H11" s="147"/>
       <c r="I11" s="169" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="J11" s="147"/>
       <c r="K11" s="147"/>
@@ -44880,10 +44881,10 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="150" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="B12" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C12" s="160">
         <v>19.95</v>
@@ -44892,15 +44893,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="152" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="F12" s="169" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="G12" s="147"/>
       <c r="H12" s="147"/>
       <c r="I12" s="169" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="J12" s="147"/>
       <c r="K12" s="147"/>
@@ -44922,10 +44923,10 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="150" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="B13" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C13" s="156">
         <v>37.9</v>
@@ -44934,10 +44935,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="152" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="F13" s="169" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="G13" s="147"/>
       <c r="H13" s="147"/>
@@ -44962,10 +44963,10 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="150" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="B14" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C14" s="156">
         <v>29.9</v>
@@ -44978,14 +44979,14 @@
         <v>https://www.amazon.de/Raspberry-Pi-v2-1-1080P-Kamera-Modul/dp/B01ER2SMHY/ref=sr_1_4?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=1LUZK9XHFS5CX&amp;keywords=raspberry+pi+camera+v2.1&amp;qid=1565008837&amp;s=gateway&amp;sprefix=raspberry+pi+camera+%2Caps%2C163&amp;sr=8-4</v>
       </c>
       <c r="F14" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G14" s="152" t="str">
         <f>HYPERLINK("https://www.reichelt.de/raspberry-pi-kamera-8mp-ir-v2-imx219pq-rasp-can-2-p170857.html?&amp;trstct=pos_2","https://www.reichelt.de/raspberry-pi-kamera-8mp-ir-v2-imx219pq-rasp-can-2-p170857.html?&amp;trstct=pos_2")</f>
         <v>https://www.reichelt.de/raspberry-pi-kamera-8mp-ir-v2-imx219pq-rasp-can-2-p170857.html?&amp;trstct=pos_2</v>
       </c>
       <c r="H14" s="169" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="I14" s="147"/>
       <c r="J14" s="147"/>
@@ -45008,10 +45009,10 @@
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="154" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="B15" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C15" s="147"/>
       <c r="D15" s="156">
@@ -45022,17 +45023,17 @@
         <v>https://www.amazon.de/gp/product/B075JN61S7/ref=ox_sc_act_title_2?smid=A1X7QLRQH87QA3&amp;psc=1</v>
       </c>
       <c r="F15" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G15" s="152" t="str">
         <f>HYPERLINK("https://www.az-delivery.de/collections/raspberry-pi-kamera-zubehor/products/100cmflexkabel?ls=de","https://www.az-delivery.de/collections/raspberry-pi-kamera-zubehor/products/100cmflexkabel?ls=de")</f>
         <v>https://www.az-delivery.de/collections/raspberry-pi-kamera-zubehor/products/100cmflexkabel?ls=de</v>
       </c>
       <c r="H15" s="147" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="I15" s="169" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="J15" s="147"/>
       <c r="K15" s="147"/>
@@ -45054,10 +45055,10 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="150" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="B16" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C16" s="156">
         <v>64.5</v>
@@ -45070,13 +45071,13 @@
         <v>https://www.amazon.de/Raspberry-Pi-7-Inch-Screen-Display/dp/B014WKCFR4/ref=sr_1_fkmrnull_3?__mk_de_DE=ÅMÅŽÕÑ&amp;keywords=raspi+7"+tft&amp;qid=1555581857&amp;s=gateway&amp;sr=8-3-fkmrnull</v>
       </c>
       <c r="F16" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G16" s="152" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="H16" s="147" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="I16" s="147"/>
       <c r="J16" s="147"/>
@@ -45099,10 +45100,10 @@
     </row>
     <row r="17" spans="1:26">
       <c r="A17" s="150" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="B17" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C17" s="156">
         <v>17.8</v>
@@ -45111,16 +45112,16 @@
         <v>1</v>
       </c>
       <c r="E17" s="152" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="F17" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G17" s="69" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="H17" s="169" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="I17" s="147"/>
       <c r="J17" s="147"/>
@@ -45143,10 +45144,10 @@
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="150" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="B18" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C18" s="156">
         <v>8.5500000000000007</v>
@@ -45155,10 +45156,10 @@
         <v>1</v>
       </c>
       <c r="E18" s="152" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="F18" s="169" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="G18" s="147"/>
       <c r="H18" s="147"/>
@@ -45183,10 +45184,10 @@
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="161" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B19" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C19" s="147"/>
       <c r="D19" s="156">
@@ -45197,10 +45198,10 @@
         <v>https://www.amazon.de/BisLinks%C2%AE-Facing-Kamera-Ersatz-Repair/dp/B01M9K9RVN/ref=sr_1_10?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=lg+g3+camera&amp;qid=1565005739&amp;s=gateway&amp;sr=8-10</v>
       </c>
       <c r="F19" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G19" s="147" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="H19" s="147"/>
       <c r="I19" s="147"/>
@@ -45224,10 +45225,10 @@
     </row>
     <row r="20" spans="1:26">
       <c r="A20" s="150" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="B20" s="151" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="C20" s="156"/>
       <c r="D20" s="156">
@@ -45238,17 +45239,17 @@
         <v>https://www.amazon.de/AZDelivery-NodeMCU-Development-Nachfolgermodell-ESP8266/dp/B074RGW2VQ/ref=sr_1_3?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=esp32&amp;qid=1565008313&amp;s=gateway&amp;sr=8-3</v>
       </c>
       <c r="F20" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G20" s="152" t="str">
         <f>HYPERLINK("https://www.az-delivery.de/products/esp32-developmentboard?ls=de","https://www.az-delivery.de/products/esp32-developmentboard?ls=de")</f>
         <v>https://www.az-delivery.de/products/esp32-developmentboard?ls=de</v>
       </c>
       <c r="H20" s="147" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="I20" s="147" t="s">
-        <v>563</v>
+        <v>552</v>
       </c>
       <c r="J20" s="147"/>
       <c r="K20" s="147"/>
@@ -45270,10 +45271,10 @@
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="171" t="s">
-        <v>564</v>
+        <v>553</v>
       </c>
       <c r="B21" s="172" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="C21" s="173"/>
       <c r="D21" s="156">
@@ -45283,12 +45284,12 @@
         <v>140</v>
       </c>
       <c r="F21" s="169" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="G21" s="147"/>
       <c r="H21" s="147"/>
       <c r="I21" s="171" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="J21" s="174"/>
       <c r="K21" s="147"/>
@@ -45310,10 +45311,10 @@
     </row>
     <row r="22" spans="1:26">
       <c r="A22" s="150" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="B22" s="151" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="C22" s="156"/>
       <c r="D22" s="156">
@@ -45324,17 +45325,17 @@
         <v>https://www.amazon.de/AZDelivery-Matrix-CJMCU-8-Arduino-Raspberry/dp/B078HYP681/ref=sr_1_2?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=neopixel+matrix&amp;qid=1565008576&amp;s=gateway&amp;sr=8-2</v>
       </c>
       <c r="F22" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G22" s="152" t="str">
         <f>HYPERLINK("https://www.az-delivery.de/products/u-64-led-panel?ls=de","https://www.az-delivery.de/products/u-64-led-panel?ls=de")</f>
         <v>https://www.az-delivery.de/products/u-64-led-panel?ls=de</v>
       </c>
       <c r="H22" s="147" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="I22" s="153" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="J22" s="175"/>
       <c r="K22" s="147"/>
@@ -45356,10 +45357,10 @@
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="147" t="s">
-        <v>569</v>
+        <v>558</v>
       </c>
       <c r="B23" s="176" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C23" s="156"/>
       <c r="D23" s="156">
@@ -45370,17 +45371,17 @@
         <v>https://www.ebay.de/itm/Hi-Power-LED-1W-3W-UV-STAR-Ultraviolet-/131326525056?var=</v>
       </c>
       <c r="F23" s="169" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="G23" s="152" t="str">
         <f>HYPERLINK("https://avonec.de/3w-high-power-led/3w-high-power-led-10000k-20000k-kaltweiss-46-47-48.html","https://avonec.de/3w-high-power-led/3w-high-power-led-10000k-20000k-kaltweiss-46-47-48.html")</f>
         <v>https://avonec.de/3w-high-power-led/3w-high-power-led-10000k-20000k-kaltweiss-46-47-48.html</v>
       </c>
       <c r="H23" s="147" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="I23" s="147" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="J23" s="177"/>
       <c r="K23" s="147"/>
@@ -45402,10 +45403,10 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="154" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="B24" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C24" s="156"/>
       <c r="D24" s="156">
@@ -45416,17 +45417,17 @@
         <v>https://www.ebay.de/itm/BD809-Transistor-npn-80V-10A-90W-TO220/360661360188?hash=item53f9179e3c:g:ssEAAOSw-fNaqt1l</v>
       </c>
       <c r="F24" s="169" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="G24" s="152" t="str">
         <f>HYPERLINK("https://www.reichelt.de/index.html?ACTION=446&amp;LA=446&amp;q=bd809%20transistor%20npn%2080v%2010a%2090w%20to220","https://www.reichelt.de/index.html?ACTION=446&amp;LA=446&amp;q=bd809%20transistor%20npn%2080v%2010a%2090w%20to220")</f>
         <v>https://www.reichelt.de/index.html?ACTION=446&amp;LA=446&amp;q=bd809%20transistor%20npn%2080v%2010a%2090w%20to220</v>
       </c>
       <c r="H24" s="169" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="I24" s="171" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="J24" s="147"/>
       <c r="K24" s="147"/>
@@ -45448,10 +45449,10 @@
     </row>
     <row r="25" spans="1:26">
       <c r="A25" s="154" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="B25" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C25" s="156"/>
       <c r="D25" s="156">
@@ -45462,16 +45463,16 @@
         <v>https://www.amazon.de/Elegoo-Stepper-Schrittmotor-28BYJ-48-Treiberplatine/dp/B01MEGIHLF/ref=sr_1_1_sspa?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=stepper+arduino&amp;qid=1565008205&amp;s=gateway&amp;sr=8-1-spons&amp;psc=1</v>
       </c>
       <c r="F25" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G25" s="152" t="s">
         <v>207</v>
       </c>
       <c r="H25" s="169" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="I25" s="171" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="J25" s="147"/>
       <c r="K25" s="147"/>
@@ -45493,10 +45494,10 @@
     </row>
     <row r="26" spans="1:26">
       <c r="A26" s="150" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="B26" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C26" s="147"/>
       <c r="D26" s="156">
@@ -45507,12 +45508,12 @@
         <v>https://eshop.wuerth.de/Zylinderschraube-mit-Innensechskant-SHR-ZYL-ISO4762-88-IS25-A2K-M3X8/00843%20%208.sku/de/DE/EUR/</v>
       </c>
       <c r="F26" s="147" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="G26" s="147"/>
       <c r="H26" s="147"/>
       <c r="I26" s="178" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="J26" s="147"/>
       <c r="K26" s="178"/>
@@ -45534,10 +45535,10 @@
     </row>
     <row r="27" spans="1:26">
       <c r="A27" s="150" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="B27" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C27" s="147"/>
       <c r="D27" s="156">
@@ -45548,12 +45549,12 @@
         <v>https://eshop.wuerth.de/Zylinderschraube-mit-Innensechskant-SHR-ZYL-ISO4762-88-IS25-A2K-M3X12/00843%20%2012.sku/de/DE/EUR/</v>
       </c>
       <c r="F27" s="147" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="G27" s="147"/>
       <c r="H27" s="147"/>
       <c r="I27" s="178" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="J27" s="147"/>
       <c r="K27" s="147"/>
@@ -45575,10 +45576,10 @@
     </row>
     <row r="28" spans="1:26">
       <c r="A28" s="161" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="B28" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C28" s="147"/>
       <c r="D28" s="156">
@@ -45589,12 +45590,12 @@
         <v>https://eshop.wuerth.de/Zylinderschraube-mit-Innensechskant-SHR-ZYL-ISO4762-88-IS25-A2K-M3X18/00843%20%2018.sku/de/DE/EUR/</v>
       </c>
       <c r="F28" s="147" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="G28" s="147"/>
       <c r="H28" s="147"/>
       <c r="I28" s="179" t="s">
-        <v>579</v>
+        <v>568</v>
       </c>
       <c r="J28" s="178"/>
       <c r="K28" s="147"/>
@@ -45616,10 +45617,10 @@
     </row>
     <row r="29" spans="1:26">
       <c r="A29" s="150" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
       <c r="B29" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C29" s="180">
         <v>0.36</v>
@@ -45632,16 +45633,16 @@
         <v>https://www.ebay.de/itm/216-Neodym-Kugelmagnete-D5mm-D7mm-D10mm-GOLD-SILVER-BLACK-NICKEL-NdFeB/372719170845?hash=item56c7cb351d:m:mj8zDp5AN1PxzUDiyJu1Rsg</v>
       </c>
       <c r="F29" s="147" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="G29" s="152" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="H29" s="147" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="I29" s="179" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="J29" s="181"/>
       <c r="K29" s="178"/>
@@ -45663,10 +45664,10 @@
     </row>
     <row r="30" spans="1:26">
       <c r="A30" s="161" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="B30" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C30" s="147"/>
       <c r="D30" s="156">
@@ -45677,7 +45678,7 @@
         <v>https://eshop.wuerth.de/Gewindestift-Innensechskant-und-Kegelstumpf-STI-STMPF-ISO4026-45H-IS15-A2K-M3X25/025503%2025.sku/WuerthGroup-Wuerth.cgid/de/DE/EUR/?VisibleSearchTerm=STI-STMPF-ISO4026-45H-IS1%2C5-%28A2K%29-M3X25&amp;CampaignName=SR001</v>
       </c>
       <c r="F30" s="147" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="G30" s="147"/>
       <c r="H30" s="147"/>
@@ -45702,20 +45703,20 @@
     </row>
     <row r="31" spans="1:26">
       <c r="A31" s="161" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
       <c r="B31" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C31" s="147"/>
       <c r="D31" s="147">
         <v>1</v>
       </c>
       <c r="E31" s="152" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="F31" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G31" s="147"/>
       <c r="H31" s="147"/>
@@ -45740,26 +45741,26 @@
     </row>
     <row r="32" spans="1:26">
       <c r="A32" s="150" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="B32" s="151" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C32" s="147"/>
       <c r="D32" s="147">
         <v>1</v>
       </c>
       <c r="E32" s="152" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="F32" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G32" s="182" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="H32" s="147" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="I32" s="147"/>
       <c r="J32" s="147"/>
@@ -45782,22 +45783,22 @@
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="169" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
       <c r="B33" s="183" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="C33" s="169"/>
       <c r="D33" s="147"/>
       <c r="E33" s="147"/>
       <c r="F33" s="169" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="G33" s="147"/>
       <c r="H33" s="147"/>
       <c r="I33" s="147"/>
       <c r="J33" s="184" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
       <c r="K33" s="147"/>
       <c r="L33" s="147"/>
@@ -45818,30 +45819,30 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="147" t="s">
+        <v>514</v>
+      </c>
+      <c r="B34" s="176" t="s">
         <v>525</v>
-      </c>
-      <c r="B34" s="176" t="s">
-        <v>536</v>
       </c>
       <c r="C34" s="147"/>
       <c r="D34" s="156">
         <v>3</v>
       </c>
       <c r="E34" s="152" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="F34" s="147" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="G34" s="147"/>
       <c r="H34" s="147"/>
       <c r="I34" s="147" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
       <c r="J34" s="181"/>
       <c r="K34" s="147"/>
       <c r="L34" s="185" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="M34" s="147"/>
       <c r="N34" s="149"/>
@@ -45860,24 +45861,24 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="179" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="B35" s="172" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C35" s="147"/>
       <c r="D35" s="147"/>
       <c r="E35" s="186" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
       <c r="F35" s="147" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="G35" s="182" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="H35" s="147" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="I35" s="147"/>
       <c r="J35" s="147"/>
@@ -45900,10 +45901,10 @@
     </row>
     <row r="36" spans="1:26">
       <c r="A36" s="154" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="B36" s="187" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="C36" s="147"/>
       <c r="D36" s="156">
@@ -45913,12 +45914,12 @@
         <v>93</v>
       </c>
       <c r="F36" s="147" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
       <c r="G36" s="147"/>
       <c r="H36" s="147"/>
       <c r="I36" s="179" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="J36" s="181"/>
       <c r="K36" s="147"/>
@@ -45940,10 +45941,10 @@
     </row>
     <row r="37" spans="1:26">
       <c r="A37" s="161" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="B37" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C37" s="147"/>
       <c r="D37" s="156">
@@ -45974,10 +45975,10 @@
     </row>
     <row r="38" spans="1:26">
       <c r="A38" s="161" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="B38" s="162" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C38" s="147"/>
       <c r="D38" s="156">
@@ -46008,7 +46009,7 @@
     </row>
     <row r="39" spans="1:26">
       <c r="A39" s="147" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="B39" s="188"/>
       <c r="C39" s="147"/>
@@ -46040,7 +46041,7 @@
     </row>
     <row r="40" spans="1:26">
       <c r="A40" s="190" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="B40" s="156"/>
       <c r="C40" s="147"/>

</xml_diff>